<commit_message>
Chapitre 4: erreurs du parser + intro nombre total trackers
</commit_message>
<xml_diff>
--- a/papier/graphiques/Analyse_40-jours.xlsx
+++ b/papier/graphiques/Analyse_40-jours.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\François\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="crawler" sheetId="1" r:id="rId1"/>
+    <sheet name="parser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -36,6 +37,18 @@
   </si>
   <si>
     <t># échecs</t>
+  </si>
+  <si>
+    <t># fichiers</t>
+  </si>
+  <si>
+    <t># succès</t>
+  </si>
+  <si>
+    <t>% succès</t>
+  </si>
+  <si>
+    <t># trackers</t>
   </si>
 </sst>
 </file>
@@ -71,9 +84,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -116,7 +130,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$B$2</c:f>
+              <c:f>crawler!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -139,7 +153,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$3:$A$42</c:f>
+              <c:f>crawler!$A$3:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="40"/>
@@ -268,7 +282,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$3:$B$42</c:f>
+              <c:f>crawler!$B$3:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -402,7 +416,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Feuil1!$C$2</c:f>
+              <c:f>crawler!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -425,7 +439,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Feuil1!$A$3:$A$42</c:f>
+              <c:f>crawler!$A$3:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="40"/>
@@ -554,7 +568,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$C$3:$C$42</c:f>
+              <c:f>crawler!$C$3:$C$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="40"/>
@@ -692,11 +706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="275450688"/>
-        <c:axId val="275451232"/>
+        <c:axId val="-255275792"/>
+        <c:axId val="-255281776"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="275450688"/>
+        <c:axId val="-255275792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,14 +753,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275451232"/>
+        <c:crossAx val="-255281776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="275451232"/>
+        <c:axId val="-255281776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,7 +811,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275450688"/>
+        <c:crossAx val="-255275792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -811,7 +825,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -841,6 +854,936 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>parser!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% succès</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>parser!$A$3:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>41726</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41729</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41731</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41733</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41734</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41735</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41736</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41738</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41739</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41740</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41742</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41743</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41744</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41745</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41746</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41747</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41748</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41749</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41750</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41751</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41752</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41753</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41754</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41755</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41756</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41757</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41758</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41759</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41760</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41761</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41762</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41763</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41764</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41765</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41766</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>parser!$D$3:$D$42</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>0.99791666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99788806758183735</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99893617021276593</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99896049896049899</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99689762150982419</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99644970414201184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99689440993788825</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99690721649484537</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99785867237687365</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99784017278617709</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99782608695652175</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9968085106382979</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99677419354838714</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99789915966386555</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99788359788359793</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99787685774946921</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99683544303797467</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99688473520249221</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99681190223166849</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99567099567099571</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99784482758620685</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99571734475374729</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99791449426485923</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99684542586750791</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.98627243928194297</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.98843322818086221</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98547717842323657</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.98540145985401462</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.98422712933753942</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.98435870698644423</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.98750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.98622881355932202</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.98824786324786329</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.98776418242491659</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.98687089715536103</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.98662207357859533</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.99239130434782608</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.98742138364779874</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.98756476683937822</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.98842105263157898</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-255270896"/>
+        <c:axId val="-255271440"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="-255270896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-255271440"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-255271440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0.98"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-255270896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>parser!$A$3:$A$42</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>41726</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41727</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41728</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41729</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41730</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41731</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41733</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41734</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41735</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41736</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41738</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41739</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41740</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41741</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41742</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41743</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41744</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41745</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41746</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41747</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41748</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41749</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41750</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41751</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41752</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41753</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41754</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41755</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41756</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41757</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41758</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41759</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41760</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41761</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41762</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41763</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41764</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41765</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41766</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>parser!$E$3:$E$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>29905</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30472</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30513</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31330</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25770</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31503</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30275</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28786</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>29612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30127</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29578</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30571</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>30468</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30669</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30888</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30407</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28813</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>29917</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>29874</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30174</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>30291</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>29793</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29963</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31088</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>30549</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29867</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31033</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31354</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30682</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>30225</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>29434</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>30545</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>29442</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28949</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>30617</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>30576</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>30193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-44264320"/>
+        <c:axId val="-44275744"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="-44264320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-44275744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="-44275744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="20000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-44264320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -918,7 +1861,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1439,15 +3494,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>7938</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1461,6 +3516,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>14188</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>728663</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Graphique 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1734,8 +3854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,4 +4324,771 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.42578125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>41726</v>
+      </c>
+      <c r="B3">
+        <v>960</v>
+      </c>
+      <c r="C3">
+        <v>958</v>
+      </c>
+      <c r="D3" s="2">
+        <f>C3/B3</f>
+        <v>0.99791666666666667</v>
+      </c>
+      <c r="E3">
+        <v>29905</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>41727</v>
+      </c>
+      <c r="B4">
+        <v>947</v>
+      </c>
+      <c r="C4">
+        <v>945</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D42" si="0">C4/B4</f>
+        <v>0.99788806758183735</v>
+      </c>
+      <c r="E4">
+        <v>30472</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>41728</v>
+      </c>
+      <c r="B5">
+        <v>940</v>
+      </c>
+      <c r="C5">
+        <v>939</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99893617021276593</v>
+      </c>
+      <c r="E5">
+        <v>28862</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>41729</v>
+      </c>
+      <c r="B6">
+        <v>962</v>
+      </c>
+      <c r="C6">
+        <v>961</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99896049896049899</v>
+      </c>
+      <c r="E6">
+        <v>30513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>41730</v>
+      </c>
+      <c r="B7">
+        <v>967</v>
+      </c>
+      <c r="C7">
+        <v>964</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99689762150982419</v>
+      </c>
+      <c r="E7">
+        <v>31330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>41731</v>
+      </c>
+      <c r="B8">
+        <v>845</v>
+      </c>
+      <c r="C8">
+        <v>842</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99644970414201184</v>
+      </c>
+      <c r="E8">
+        <v>25770</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>41732</v>
+      </c>
+      <c r="B9">
+        <v>966</v>
+      </c>
+      <c r="C9">
+        <v>963</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99689440993788825</v>
+      </c>
+      <c r="E9">
+        <v>31503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>41733</v>
+      </c>
+      <c r="B10">
+        <v>970</v>
+      </c>
+      <c r="C10">
+        <v>967</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99690721649484537</v>
+      </c>
+      <c r="E10">
+        <v>30275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>41734</v>
+      </c>
+      <c r="B11">
+        <v>934</v>
+      </c>
+      <c r="C11">
+        <v>932</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99785867237687365</v>
+      </c>
+      <c r="E11">
+        <v>29875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>41735</v>
+      </c>
+      <c r="B12">
+        <v>926</v>
+      </c>
+      <c r="C12">
+        <v>924</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99784017278617709</v>
+      </c>
+      <c r="E12">
+        <v>28786</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>41736</v>
+      </c>
+      <c r="B13">
+        <v>920</v>
+      </c>
+      <c r="C13">
+        <v>918</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99782608695652175</v>
+      </c>
+      <c r="E13">
+        <v>29612</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>41738</v>
+      </c>
+      <c r="B14">
+        <v>940</v>
+      </c>
+      <c r="C14">
+        <v>937</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9968085106382979</v>
+      </c>
+      <c r="E14">
+        <v>30179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>41739</v>
+      </c>
+      <c r="B15">
+        <v>930</v>
+      </c>
+      <c r="C15">
+        <v>927</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99677419354838714</v>
+      </c>
+      <c r="E15">
+        <v>30127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>41740</v>
+      </c>
+      <c r="B16">
+        <v>952</v>
+      </c>
+      <c r="C16">
+        <v>950</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99789915966386555</v>
+      </c>
+      <c r="E16">
+        <v>29578</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>41741</v>
+      </c>
+      <c r="B17">
+        <v>945</v>
+      </c>
+      <c r="C17">
+        <v>943</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99788359788359793</v>
+      </c>
+      <c r="E17">
+        <v>30571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>41742</v>
+      </c>
+      <c r="B18">
+        <v>942</v>
+      </c>
+      <c r="C18">
+        <v>940</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99787685774946921</v>
+      </c>
+      <c r="E18">
+        <v>30468</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>41743</v>
+      </c>
+      <c r="B19">
+        <v>948</v>
+      </c>
+      <c r="C19">
+        <v>945</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99683544303797467</v>
+      </c>
+      <c r="E19">
+        <v>30669</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>41744</v>
+      </c>
+      <c r="B20">
+        <v>963</v>
+      </c>
+      <c r="C20">
+        <v>960</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99688473520249221</v>
+      </c>
+      <c r="E20">
+        <v>30888</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>41745</v>
+      </c>
+      <c r="B21">
+        <v>941</v>
+      </c>
+      <c r="C21">
+        <v>938</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99681190223166849</v>
+      </c>
+      <c r="E21">
+        <v>30407</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>41746</v>
+      </c>
+      <c r="B22">
+        <v>924</v>
+      </c>
+      <c r="C22">
+        <v>920</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99567099567099571</v>
+      </c>
+      <c r="E22">
+        <v>28813</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>41747</v>
+      </c>
+      <c r="B23">
+        <v>928</v>
+      </c>
+      <c r="C23">
+        <v>926</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99784482758620685</v>
+      </c>
+      <c r="E23">
+        <v>29917</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>41748</v>
+      </c>
+      <c r="B24">
+        <v>934</v>
+      </c>
+      <c r="C24">
+        <v>930</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99571734475374729</v>
+      </c>
+      <c r="E24">
+        <v>29874</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>41749</v>
+      </c>
+      <c r="B25">
+        <v>959</v>
+      </c>
+      <c r="C25">
+        <v>957</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99791449426485923</v>
+      </c>
+      <c r="E25">
+        <v>30174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>41750</v>
+      </c>
+      <c r="B26">
+        <v>951</v>
+      </c>
+      <c r="C26">
+        <v>948</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99684542586750791</v>
+      </c>
+      <c r="E26">
+        <v>30291</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>41751</v>
+      </c>
+      <c r="B27">
+        <v>947</v>
+      </c>
+      <c r="C27">
+        <v>934</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98627243928194297</v>
+      </c>
+      <c r="E27">
+        <v>29793</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>41752</v>
+      </c>
+      <c r="B28">
+        <v>951</v>
+      </c>
+      <c r="C28">
+        <v>940</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98843322818086221</v>
+      </c>
+      <c r="E28">
+        <v>29963</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>41753</v>
+      </c>
+      <c r="B29">
+        <v>964</v>
+      </c>
+      <c r="C29">
+        <v>950</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98547717842323657</v>
+      </c>
+      <c r="E29">
+        <v>31088</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>41754</v>
+      </c>
+      <c r="B30">
+        <v>959</v>
+      </c>
+      <c r="C30">
+        <v>945</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98540145985401462</v>
+      </c>
+      <c r="E30">
+        <v>30549</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>41755</v>
+      </c>
+      <c r="B31">
+        <v>951</v>
+      </c>
+      <c r="C31">
+        <v>936</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98422712933753942</v>
+      </c>
+      <c r="E31">
+        <v>29867</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>41756</v>
+      </c>
+      <c r="B32">
+        <v>959</v>
+      </c>
+      <c r="C32">
+        <v>944</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98435870698644423</v>
+      </c>
+      <c r="E32">
+        <v>31033</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>41757</v>
+      </c>
+      <c r="B33">
+        <v>960</v>
+      </c>
+      <c r="C33">
+        <v>948</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="E33">
+        <v>31354</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>41758</v>
+      </c>
+      <c r="B34">
+        <v>944</v>
+      </c>
+      <c r="C34">
+        <v>931</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98622881355932202</v>
+      </c>
+      <c r="E34">
+        <v>30682</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>41759</v>
+      </c>
+      <c r="B35">
+        <v>936</v>
+      </c>
+      <c r="C35">
+        <v>925</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98824786324786329</v>
+      </c>
+      <c r="E35">
+        <v>30225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>41760</v>
+      </c>
+      <c r="B36">
+        <v>899</v>
+      </c>
+      <c r="C36">
+        <v>888</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98776418242491659</v>
+      </c>
+      <c r="E36">
+        <v>29434</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>41761</v>
+      </c>
+      <c r="B37">
+        <v>914</v>
+      </c>
+      <c r="C37">
+        <v>902</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98687089715536103</v>
+      </c>
+      <c r="E37">
+        <v>30545</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>41762</v>
+      </c>
+      <c r="B38">
+        <v>897</v>
+      </c>
+      <c r="C38">
+        <v>885</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98662207357859533</v>
+      </c>
+      <c r="E38">
+        <v>29442</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>41763</v>
+      </c>
+      <c r="B39">
+        <v>920</v>
+      </c>
+      <c r="C39">
+        <v>913</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.99239130434782608</v>
+      </c>
+      <c r="E39">
+        <v>28949</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>41764</v>
+      </c>
+      <c r="B40">
+        <v>954</v>
+      </c>
+      <c r="C40">
+        <v>942</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98742138364779874</v>
+      </c>
+      <c r="E40">
+        <v>30617</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>41765</v>
+      </c>
+      <c r="B41">
+        <v>965</v>
+      </c>
+      <c r="C41">
+        <v>953</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98756476683937822</v>
+      </c>
+      <c r="E41">
+        <v>30576</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41766</v>
+      </c>
+      <c r="B42">
+        <v>950</v>
+      </c>
+      <c r="C42">
+        <v>939</v>
+      </c>
+      <c r="D42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.98842105263157898</v>
+      </c>
+      <c r="E42">
+        <v>30193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f>AVERAGE(E3:E42)</f>
+        <v>30079.224999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mise à jour graphiques expérience 40 jours
</commit_message>
<xml_diff>
--- a/papier/graphiques/Analyse_40-jours.xlsx
+++ b/papier/graphiques/Analyse_40-jours.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Documents\thesis\papier\graphiques\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="crawler" sheetId="1" r:id="rId1"/>
-    <sheet name="parser" sheetId="2" r:id="rId2"/>
+    <sheet name="Graphique3" sheetId="5" r:id="rId1"/>
+    <sheet name="crawler" sheetId="1" r:id="rId2"/>
+    <sheet name="Graphique1" sheetId="3" r:id="rId3"/>
+    <sheet name="Graphique2" sheetId="4" r:id="rId4"/>
+    <sheet name="parser" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -706,16 +709,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-255275792"/>
-        <c:axId val="-255281776"/>
+        <c:axId val="204481136"/>
+        <c:axId val="204478392"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-255275792"/>
+        <c:axId val="204481136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Jour d'analyse</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -738,7 +797,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -753,14 +812,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-255281776"/>
+        <c:crossAx val="204478392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-255281776"/>
+        <c:axId val="204478392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -780,6 +839,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Nombre</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800" baseline="0"/>
+                  <a:t> de s</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>ites en échec</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -796,7 +919,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -811,7 +934,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-255275792"/>
+        <c:crossAx val="204481136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -825,6 +948,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -838,7 +962,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -883,11 +1007,6 @@
       <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1206,16 +1325,77 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-255270896"/>
-        <c:axId val="-255271440"/>
+        <c:axId val="172326200"/>
+        <c:axId val="172325024"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-255270896"/>
+        <c:axId val="172326200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Jour</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800" baseline="0"/>
+                  <a:t> d'analyse</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-BE" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1238,7 +1418,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1253,14 +1433,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-255271440"/>
+        <c:crossAx val="172325024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-255271440"/>
+        <c:axId val="172325024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1282,6 +1462,75 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Pourcentage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800" baseline="0"/>
+                  <a:t> de f</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>ichiers</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800" baseline="0"/>
+                  <a:t> correctement analysés</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-BE" sz="1800"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1298,7 +1547,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1313,7 +1562,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-255270896"/>
+        <c:crossAx val="172326200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1354,11 +1603,6 @@
       <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1666,16 +1910,72 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-44264320"/>
-        <c:axId val="-44275744"/>
+        <c:axId val="170736384"/>
+        <c:axId val="204481920"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-44264320"/>
+        <c:axId val="170736384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Jour d'analyse</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1698,7 +1998,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1713,14 +2013,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-44275744"/>
+        <c:crossAx val="204481920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-44275744"/>
+        <c:axId val="204481920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20000"/>
@@ -1741,6 +2041,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-BE" sz="1800"/>
+                  <a:t>Nombre total de trackers</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1757,7 +2113,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1772,7 +2128,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-44264320"/>
+        <c:crossAx val="170736384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1813,11 +2169,6 @@
       <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3489,25 +3840,50 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="70" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="70" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="70" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>7938</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310221" cy="6079191"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3520,29 +3896,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>4761</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>14188</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310221" cy="6079191"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Graphique 2"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3555,24 +3923,21 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>728663</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>28574</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9310221" cy="6079191"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Graphique 3"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3580,12 +3945,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3854,9 +4219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4322,7 +4685,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4330,7 +4692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -5089,6 +5451,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Images en noir et blanc + remerciements
</commit_message>
<xml_diff>
--- a/papier/graphiques/Analyse_40-jours.xlsx
+++ b/papier/graphiques/Analyse_40-jours.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antoine\Documents\thesis\papier\graphiques\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\graphiques\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Graphique3" sheetId="5" r:id="rId1"/>
@@ -147,6 +147,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -709,11 +710,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="204481136"/>
-        <c:axId val="204478392"/>
+        <c:axId val="147088816"/>
+        <c:axId val="147096696"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="204481136"/>
+        <c:axId val="147088816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,14 +813,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204478392"/>
+        <c:crossAx val="147096696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="204478392"/>
+        <c:axId val="147096696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,7 +935,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204481136"/>
+        <c:crossAx val="147088816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1325,11 +1326,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="172326200"/>
-        <c:axId val="172325024"/>
+        <c:axId val="146978816"/>
+        <c:axId val="146577160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="172326200"/>
+        <c:axId val="146978816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1366,7 +1367,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1433,14 +1433,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172325024"/>
+        <c:crossAx val="146577160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="172325024"/>
+        <c:axId val="146577160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1501,7 +1501,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1562,7 +1561,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="172326200"/>
+        <c:crossAx val="146978816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1910,11 +1909,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="170736384"/>
-        <c:axId val="204481920"/>
+        <c:axId val="146786184"/>
+        <c:axId val="146786568"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="170736384"/>
+        <c:axId val="146786184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1946,7 +1945,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2013,14 +2011,14 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="204481920"/>
+        <c:crossAx val="146786568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="204481920"/>
+        <c:axId val="146786568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="20000"/>
@@ -2067,7 +2065,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2128,7 +2125,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="170736384"/>
+        <c:crossAx val="146786184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3844,7 +3841,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3877,7 +3874,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9310221" cy="6079191"/>
+    <xdr:ext cx="9293679" cy="6068786"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1"/>
@@ -4219,7 +4216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>